<commit_message>
Updated analysis with new files and modifications
</commit_message>
<xml_diff>
--- a/colored_word_pairs.xlsx
+++ b/colored_word_pairs.xlsx
@@ -26,46 +26,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color rgb="00FF6384"/>
+    </font>
+    <font>
+      <color rgb="0036A2EB"/>
+    </font>
+    <font>
+      <color rgb="00FFCE56"/>
+    </font>
+    <font>
+      <color rgb="004BC0C0"/>
+    </font>
+    <font>
+      <color rgb="009966FF"/>
+    </font>
+    <font>
+      <color rgb="00FF9F40"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="0036A2EB"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFCE56"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="004BC0C0"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="009966FF"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FF9F40"/>
+    </font>
+    <font>
       <b val="1"/>
       <color rgb="00FF6384"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="0036A2EB"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFCE56"/>
-    </font>
-    <font>
-      <color rgb="004BC0C0"/>
-    </font>
-    <font>
-      <color rgb="009966FF"/>
-    </font>
-    <font>
-      <color rgb="00FF9F40"/>
-    </font>
-    <font>
-      <color rgb="00FF6384"/>
-    </font>
-    <font>
-      <color rgb="0036A2EB"/>
-    </font>
-    <font>
-      <color rgb="00FFCE56"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="004BC0C0"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="009966FF"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FF9F40"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,16 +88,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -463,7 +464,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,24 +487,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bajta - Britto_2016</t>
+          <t>Bajta - Britto_2017</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>estimated value - estimator - temporal distance</t>
+          <t>risk - risk level - hardware - technical factors - platform support level - design - architecture - maintainability - portability level - installability level - maintainability level - reliability level - reusability level - size report - team size - performance - time efficiency level - process efficiency level - quality level - availability - availability level - individual - personality - security - security level - reliability - robustness level - testing - testability level - effort hours - maintenance - no of team members - team capability - work team level</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bajta - Britto_2017</t>
+          <t>Bajta - Britto_2016</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>reliability - reliability level - risk - risk level - number of team members - team size - maintainability - maintainability level - security - security level - availability - availability level</t>
+          <t>estimate value - estimator &amp; provider - estimator - temporal distance - relationship.geographic distance - site.temporal distance - relationship.temporal distance - geographical distance - site.geographic distance</t>
         </is>
       </c>
     </row>
@@ -515,55 +516,55 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>expert judgment - cocomo</t>
+          <t>constructive cost model - fuzzy similar - fuzzy logic - expert judgment - machine learning - artificial neural networks</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bajta - Usman</t>
+          <t>Bajta - Mendes</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>reliability - maintainability - analysis - near offshore - far offshore - close onshore - distant onshore - number of team members - no. of team members - performance - finance - financial - value - expert judgment - expert judgement - maintenance - security - healthcare - health - not considered - not applicable - considered - estimated value - estimate value(s) - availability - testing - design - bidding - statistical analysis - implementation</t>
+          <t>not considered - validated theoretically - size report - early size metric - late size metric - implementation - functionality - performance - considered</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Britto_2016 - Bajta</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>estimator - estimated value - temporal distance</t>
+          <t>Bajta - Usman</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>estimate value - estimation entity.other - number of entities estimated.value - estimation techniques.other - estimate value(s) - actual effort.value - not considered - not used - considered - not applicable - agile - customized scrum - scrum - group-based estimation - telecommunication - communications industry - near offshore - distributed: far offshore - distributed: distant onshore - distributed: near offshore - distributed: close onshore - design - maintainability - availability - reliability - maintenance - healthcare - health - size report - size.other - implementation - performance - analysis - execution - task - finance - financial - statistics analysis - individual - single - security - other - project domain.other - unit.other - se - value - system investigation - far offshore - expert judgment - expert judgement - close onshore - testing - effort hours - ideal hours - effort estimate.type.other - hours/days - distant onshore - no of team members - no. of team members</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Britto_2016 - Usman</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>distributed - distribution - estimator - estimate value(s)</t>
+          <t>Britto_2017 - Bajta</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>technical factors - hardware - portability level - maintainability - risk level - risk - team capability - no of team members - time efficiency level - performance - effort hours - work team level - architecture - design - process efficiency level - availability level - availability - testability level - testing - personality - individual - robustness level - reliability - installability level - team size - size report - security level - security - quality level - maintainability level - maintenance - platform support level - reliability level - reusability level</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Britto_2017 - Bajta</t>
-        </is>
-      </c>
-      <c r="B8" s="6" t="inlineStr">
-        <is>
-          <t>team size - number of team members - security level - security - risk level - risk - maintainability level - maintainability - reliability level - reliability - availability level - availability</t>
+          <t>Britto_2017 - Dasthi</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>software development experience - software life cycle management</t>
         </is>
       </c>
     </row>
@@ -573,9 +574,9 @@
           <t>Britto_2017 - Mendes</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>total complexity - complexity - class complexity - component complexity - output complexity - media allocation - media - input complexity - cyclomatic complexity - media count - new complexity</t>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>interface complexity - complexity - control flow complexity - media count - media - web page allocation - web application - project.type - model dependency.specific - adaptation complexity - program count - program/script - class complexity - class.length - cyclomatic complexity - web objects - web software application - web hypermedia application - model collection complexity - difficulty level - data flow complexity - motivation level - motivation - data usage complexity - new media count - media allocation - cohesion complexity - page complexity - output complexity - new complexity - input complexity - component complexity - model association complexity - total complexity - media duration - layout complexity</t>
         </is>
       </c>
     </row>
@@ -585,117 +586,165 @@
           <t>Britto_2017 - Usman</t>
         </is>
       </c>
-      <c r="B10" s="6" t="inlineStr">
-        <is>
-          <t>team size - no. of team members - security level - security - maintainability level - maintainability - reliability level - reliability - availability level - availability</t>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>entity count - estimation entity.other - number of entities estimated.value - portability level - maintainability - project.infrastructure - project domain.other - team capability - no. of team members - project.type - effort estimate.type.other - time efficiency level - performance - work team level - time restriction - hours/days - use case count - use case - use case points method - not used - user case points - requirements novelty level - non functional requirements.other - data web points - point - international function point users group - function points - architecture - design - requirements clarity level - process efficiency level - availability level - availability - testability level - testing - processing requirements - object-oriented function points - requirements volatility level - robustness level - reliability - installability level - implementation - team size - security level - security - quality level - accuracy level.value - object-oriented heuristic function points - maintainability level - maintenance - reliability level - reusability level</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Dasthi - Bajta</t>
-        </is>
-      </c>
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>cocomo - expert judgment</t>
+          <t>Britto_2016 - Bajta</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>estimator &amp; provider - estimate value - relationship.geographic distance - temporal distance - geographical distance - site.geographic distance - estimator - site.temporal distance - relationship.temporal distance</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dasthi - Usman</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>analogy base - analogy - expert judgment - expert judgement</t>
+          <t>Britto_2016 - Usman</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>semi-distributed - distributed: far offshore - distributed: near offshore - distribution - estimator &amp; provider - estimation entity.other - estimation techniques.other - estimate value(s) - relationship.location - co-located - centralized - estimator - distributed - distributed: distant onshore - distributed: close onshore</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Mendes - Britto_2017</t>
-        </is>
-      </c>
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>media - media allocation - media count - complexity - total complexity - class complexity - component complexity - output complexity - input complexity - cyclomatic complexity - new complexity</t>
+          <t>Dasthi - Bajta</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>expert judgment - constructive cost model - artificial neural networks - machine learning - fuzzy logic - fuzzy similar</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Mendes - Usman</t>
+          <t>Dasthi - Britto_2017</t>
         </is>
       </c>
       <c r="B14" s="8" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>software life cycle management - software development experience</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Usman - Bajta</t>
-        </is>
-      </c>
-      <c r="B15" s="8" t="inlineStr">
-        <is>
-          <t>far offshore - near offshore - distant onshore - reliability - maintainability - close onshore - health - healthcare - analysis - statistical analysis - financial - finance - performance - value - maintenance - security - expert judgement - expert judgment - not applicable - not considered - no. of team members - number of team members - availability - testing - design - implementation - estimate value(s) - estimated value - considered - bidding</t>
+          <t>Dasthi - Usman</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>expert judgment - expert judgement - analogy-based - analogy</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Usman - Britto_2016</t>
+          <t>Mendes - Bajta</t>
         </is>
       </c>
       <c r="B16" s="6" t="inlineStr">
         <is>
-          <t>distribution - distributed - estimate value(s) - estimator</t>
+          <t>validated theoretically - not considered - considered - functionality - implementation - performance - early size metric - size report - late size metric</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Usman - Britto_2017</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>reliability - reliability level - maintainability - maintainability level - security - security level - no. of team members - team size - availability - availability level</t>
+          <t>Mendes - Britto_2017</t>
+        </is>
+      </c>
+      <c r="B17" s="8" t="inlineStr">
+        <is>
+          <t>web software application - web objects - motivation - motivation level - program/script - program count - web hypermedia application - complexity - interface complexity - control flow complexity - adaptation complexity - class complexity - cyclomatic complexity - model collection complexity - difficulty level - data flow complexity - data usage complexity - cohesion complexity - page complexity - output complexity - new complexity - input complexity - component complexity - model association complexity - total complexity - layout complexity - model dependency.specific - project.type - class.length - web application - web page allocation - media - media count - new media count - media allocation - media duration</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Usman - Dasthi</t>
-        </is>
-      </c>
-      <c r="B18" s="7" t="inlineStr">
-        <is>
-          <t>analogy - analogy base - expert judgement - expert judgment</t>
+          <t>Mendes - Usman</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="inlineStr">
+        <is>
+          <t>validated theoretically - not considered - considered - functionality - use case - maintainability - task - implementation - non functional requirements.other - performance - solution-oriented metric - considered without any metric - early size metric - size.other - problem-oriented metric - late size metric</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>Usman - Bajta</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>ideal hours - effort hours - size.other - size report - other - effort estimate.type.other - no. of team members - no of team members - not considered - considered - se - distributed: far offshore - near offshore - far offshore - distant onshore - distributed: distant onshore - close onshore - customized scrum - agile - maintainability - availability - reliability - maintenance - design - hours/days - task - execution - distributed: near offshore - communications industry - telecommunication - implementation - performance - project domain.other - estimation entity.other - estimate value - analysis - number of entities estimated.value - estimation techniques.other - group-based estimation - not used - statistics analysis - system investigation - distributed: close onshore - security - unit.other - expert judgement - expert judgment - estimate value(s) - value - single - individual - health - healthcare - financial - finance - not applicable - testing - scrum - actual effort.value</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Usman - Britto_2017</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>effort estimate.type.other - project.type - use case - use case count - no. of team members - team capability - work team level - team size - use case points method - function points - international function point users group - object-oriented function points - object-oriented heuristic function points - point - data web points - maintainability - portability level - installability level - maintainability level - reliability level - reusability level - design - architecture - hours/days - time restriction - accuracy level.value - quality level - implementation - non functional requirements.other - requirements novelty level - requirements clarity level - processing requirements - requirements volatility level - project domain.other - project.infrastructure - estimation entity.other - entity count - performance - time efficiency level - process efficiency level - number of entities estimated.value - not used - availability - availability level - security - security level - reliability - robustness level - user case points - testing - testability level - maintenance</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Usman - Britto_2016</t>
+        </is>
+      </c>
+      <c r="B21" s="9" t="inlineStr">
+        <is>
+          <t>distributed: far offshore - semi-distributed - distributed - distributed: distant onshore - co-located - relationship.location - centralized - distributed: near offshore - estimation entity.other - estimator &amp; provider - estimator - distribution - estimation techniques.other - distributed: close onshore - estimate value(s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Usman - Dasthi</t>
+        </is>
+      </c>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>analogy - analogy-based - expert judgement - expert judgment</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>Usman - Mendes</t>
         </is>
       </c>
-      <c r="B19" s="8" t="inlineStr">
-        <is>
-          <t>other</t>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>size.other - early size metric - late size metric - use case - functionality - not considered - validated theoretically - maintainability - task - implementation - non functional requirements.other - performance - considered - considered without any metric - solution-oriented metric - problem-oriented metric</t>
         </is>
       </c>
     </row>

</xml_diff>